<commit_message>
Updates cn2022 copy and Chapter 04.xlsx file
</commit_message>
<xml_diff>
--- a/public/cn2021_2022/2022 10 digit codes Chapter 04.xlsx
+++ b/public/cn2021_2022/2022 10 digit codes Chapter 04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc-my.sharepoint.com/personal/david_harris2_hmrc_gov_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattlavis/sites and projects/1. Online Tariff/ott prototype/app/assets/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{6AFD1FDB-ACFD-4A9E-824F-B504CCD7556B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8210B461-5A83-4CCC-9F48-58A2DBB872D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F94B5CF-E271-4749-974E-D427B7E2CB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{11520902-F9DB-49EC-8626-B124C706BFEF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" xr2:uid="{11520902-F9DB-49EC-8626-B124C706BFEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>10 Digit Codes Introduced from 1 January 2022</t>
   </si>
@@ -73,9 +73,6 @@
 - 10 % or more but not more than 30 % of blended, aged spray dried cheese,
 - 5 % or more but not more than 15 % of buttermilk and
 - 0.1 % or more but not more than 10 % of sodium caseinate, disodium phosphate, lactic acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0403 9099 39 </t>
   </si>
   <si>
     <t>10 Digit Codes Deleted from 1 January 2022</t>
@@ -678,200 +675,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D30D5F-2C55-405C-89F0-7555CE4C6800}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.59765625" customWidth="1"/>
-    <col min="2" max="2" width="70.59765625" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="6" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
+      <c r="B19" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="6" t="s">
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="6" t="s">
+      <c r="B22" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" ht="26" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" ht="26" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>3</v>
       </c>
@@ -882,7 +879,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>4</v>
       </c>
@@ -893,9 +890,9 @@
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>7</v>
@@ -904,7 +901,7 @@
       <c r="D27" s="11"/>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="1:5" ht="93" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" ht="104" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>8</v>
       </c>
@@ -912,7 +909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>9</v>
       </c>
@@ -920,63 +917,63 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" s="16" t="s">
+      <c r="B31" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B32" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" s="16" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B33" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="93" x14ac:dyDescent="0.45">
-      <c r="A36" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>50</v>
       </c>
@@ -984,27 +981,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B38" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="19" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>